<commit_message>
First Functionality ETL version
</commit_message>
<xml_diff>
--- a/models/files/dummy.xlsx
+++ b/models/files/dummy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/galigaribaldi/Documents/PPropios/UpperQuizz-API/models/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA90DD7A-B9DF-CB48-AD38-44D3BF5F8D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A482E1-46CD-BB4E-A18D-A5DD69B51610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67200" yWindow="4520" windowWidth="22040" windowHeight="14340" activeTab="3" xr2:uid="{C6ED42EB-E019-A047-9D6D-B016AF8D00A4}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="1387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1737" uniqueCount="1430">
   <si>
     <t>nombre</t>
   </si>
@@ -4326,7 +4326,136 @@
     <t>Opcion_4</t>
   </si>
   <si>
-    <t>La antropología filosófica se distingue de la antropología científica en que no toma al hombre solamente como ser natural, sino además como ser espiritual. Por lo tanto se puede decir que la antropología filosófica y la antropología científica</t>
+    <t>Giordano  Bruno  sostiene  que  lo  que  se  entiende  por  bello  depende  de  la  apreciación  particular  del  individuo. Incluso sus valoraciones estéticas pueden variar según los cambios de su estado anímico. De lo anterior se deduce que</t>
+  </si>
+  <si>
+    <t>la psicología demuestra la imposibilidad del arte y la inexistencia de la belleza.</t>
+  </si>
+  <si>
+    <t>o bello carece de una significación única válida para todos los seres humanos</t>
+  </si>
+  <si>
+    <t>la psicología puede definir la belleza a partir del análisis del individuo</t>
+  </si>
+  <si>
+    <t>lo que se conoce como belleza es simplemente un estado psicológico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La estética, en el sentido de discurso filosófico aplicado al arte y a sus relaciones con el bien y el mal, es decir, aplicado a su finalidad, se remonta a Platón. Pero gracia a Croce, tiende a desarrollarse como disciplina autónoma. De lo anterior podemos deducir que la estética como discurso filosófico ha evoluciona, porque </t>
+  </si>
+  <si>
+    <t>el arte ha sido abordado desde diferentes corrientes filosóficas</t>
+  </si>
+  <si>
+    <t>sus problemas han sido separados de otras problemáticas filosóficas</t>
+  </si>
+  <si>
+    <t>el pensamiento filosófico hace referencia a los tratados estéticos</t>
+  </si>
+  <si>
+    <t>la estética como finalidad ha buscado encontrar el sentido de la vida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para  Sartre,  la  libertad  humana  es  la  facultad  de  hacer  lo  que  uno  quiera  sin  ninguna  limitación.  La  libertad formalmente  no  tiene  ningún  contenido  determinante,  no  está  sometida  a  ninguna  necesidad  o  ley.  Sin  embargo, Sartre afirma que la libertad es una condena, porque </t>
+  </si>
+  <si>
+    <t>la única forma de limitarla es haciendo una consideración formal de la norma</t>
+  </si>
+  <si>
+    <t>exige del hombre madurez frente a la forma en la que elige su modo de actuar</t>
+  </si>
+  <si>
+    <t>ella lleva la moralidad al establecimiento de los límites</t>
+  </si>
+  <si>
+    <t>Karl Philipp Moritz escribió en 1785 que lo bello tiene una finalidad interna que consiste en provocar placer por su perfección. Esto quiere decir, que del mismo modo como a la técnica le corresponde una finalidad externa que es la utilidad, las bellas artes tienen como objetivo último el placer. Según lo anterior</t>
+  </si>
+  <si>
+    <t>una obra de arte es perfecta cuando se percibe su imagen real</t>
+  </si>
+  <si>
+    <t>la contemplación de la belleza provoca un gozo profundo</t>
+  </si>
+  <si>
+    <t>se halla gozo tanto en lo bello como en lo útil</t>
+  </si>
+  <si>
+    <t>el arte viene dado por la imitación de la naturaleza que le sirve al hombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Según Hegel, el estudio de lo bello como objeto del arte es un estudio independiente del estudio de la naturaleza. La creación artística no puede estudiarse como una rama de la ciencia natural. En otras palabras, la belleza artística es independiente de la belleza en la naturaleza. De acuerdo con lo anterior, Hegel critica  </t>
+  </si>
+  <si>
+    <t>la concepción según la cual el estudio del arte y el estudio de la naturaleza son independientes</t>
+  </si>
+  <si>
+    <t>todo intento de separar la estética de la ciencia natural</t>
+  </si>
+  <si>
+    <t>toda concepción que subordine el arte al estudio de la naturaleza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la concepción de belleza en el arte como algo independiente de lo bello natural </t>
+  </si>
+  <si>
+    <t>Algunos afirman que en los siglos XVII y XVIII, se creía que el arte y la estética gozaban de una condición interna similar a la de la naturaleza, porque</t>
+  </si>
+  <si>
+    <t>el arte es imitación de la naturaleza y por lo tanto, se rige por leyes similares</t>
+  </si>
+  <si>
+    <t>las leyes de la estética también se subordinan a un único principio que es el de la imitación</t>
+  </si>
+  <si>
+    <t>el arte es obra humana y por lo tanto, se rige por los mismos principios que rigen la ciencia</t>
+  </si>
+  <si>
+    <t>para poder plasmar la complejidad de la naturaleza, es necesario conocer sus leyes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para Descartes, la certeza en el conocimiento era fundamental, razón por la cual sometió al análisis de la razón no sólo a la filosofía, ala lógica, a la física y a la psicología, sino también al arte. Por lo tanto, se puede afirmar que para Descartes  </t>
+  </si>
+  <si>
+    <t>el arte debía cumplir con las pruebas de la razón para demostrar su verdad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">era necesario un análisis del arte para ver si su contenido era verdadero y esencial </t>
+  </si>
+  <si>
+    <t>los principios del arte eran absolutamente racionales e inamovibles</t>
+  </si>
+  <si>
+    <t>se debía realizar una crítica del arte para saber si era ciencia</t>
+  </si>
+  <si>
+    <t>Schelling muestra cómo a través del arte se pone al descubierto el interior del filósofo, mostrando que en el arte y en las creaciones artísticas tienen su encuentro la naturaleza y el espíritu, la ley y la libertad, el cuerpo y el alma, y que el filósofo se descubre en el arte cuando</t>
+  </si>
+  <si>
+    <t>reconoce en lo bello la infinitud propia del alma</t>
+  </si>
+  <si>
+    <t>su obra lo lleva a la liberación total y a la participación de lo que traspasa los límites</t>
+  </si>
+  <si>
+    <t>se reconoce como creador de una obra que se constituye en símbolo del infinito</t>
+  </si>
+  <si>
+    <t>hace descender lo infinito a la finitud a través del símbolo</t>
+  </si>
+  <si>
+    <t>Según Aristóteles “la poesía es más filosófica que la historia”. En efecto, la historia narra lo que ha sucedido. En cambio, la poesía cuenta lo que siempre puede suceder; nos enseña a ver lo universal en el obrar humano y cómo la filosofía expresa las inquietudes fundamentales del hombre. Esto significa que</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la filosofía debería guiarse por la poesía </t>
+  </si>
+  <si>
+    <t xml:space="preserve">la poesía guarda en sí una perspectiva filosófica, porque se interroga por lo universal </t>
+  </si>
+  <si>
+    <t>la historia sólo es un recuento de hechos sin interrogarse sobre el significado del obrar</t>
+  </si>
+  <si>
+    <t>la historia debería hacerse más poética</t>
   </si>
 </sst>
 </file>
@@ -6033,11 +6162,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC73719-E545-7E43-87DD-B9D8F595E672}">
-  <dimension ref="A1:L273"/>
+  <dimension ref="A1:L301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A272" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B273" sqref="B273"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -16380,12 +16507,1106 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="2:3">
+    <row r="273" spans="1:12" ht="18">
+      <c r="A273">
+        <v>272</v>
+      </c>
       <c r="B273" t="s">
         <v>1386</v>
       </c>
       <c r="C273">
         <v>10</v>
+      </c>
+      <c r="D273">
+        <v>2</v>
+      </c>
+      <c r="E273" t="s">
+        <v>1387</v>
+      </c>
+      <c r="F273" t="b">
+        <v>0</v>
+      </c>
+      <c r="G273" t="s">
+        <v>1388</v>
+      </c>
+      <c r="H273" t="b">
+        <v>1</v>
+      </c>
+      <c r="I273" t="s">
+        <v>1389</v>
+      </c>
+      <c r="J273" t="b">
+        <v>0</v>
+      </c>
+      <c r="K273" s="2" t="s">
+        <v>1390</v>
+      </c>
+      <c r="L273" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:12" ht="18">
+      <c r="A274">
+        <v>273</v>
+      </c>
+      <c r="B274" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C274">
+        <v>10</v>
+      </c>
+      <c r="D274">
+        <v>3</v>
+      </c>
+      <c r="E274" t="s">
+        <v>1392</v>
+      </c>
+      <c r="F274" t="b">
+        <v>1</v>
+      </c>
+      <c r="G274" t="s">
+        <v>1393</v>
+      </c>
+      <c r="H274" t="b">
+        <v>0</v>
+      </c>
+      <c r="I274" t="s">
+        <v>1394</v>
+      </c>
+      <c r="J274" t="b">
+        <v>0</v>
+      </c>
+      <c r="K274" s="2" t="s">
+        <v>1395</v>
+      </c>
+      <c r="L274" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:12">
+      <c r="A275">
+        <v>274</v>
+      </c>
+      <c r="B275" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C275">
+        <v>10</v>
+      </c>
+      <c r="D275">
+        <v>4</v>
+      </c>
+      <c r="E275" t="s">
+        <v>1397</v>
+      </c>
+      <c r="F275" t="b">
+        <v>0</v>
+      </c>
+      <c r="G275" t="s">
+        <v>1398</v>
+      </c>
+      <c r="H275" t="b">
+        <v>0</v>
+      </c>
+      <c r="I275" t="s">
+        <v>1399</v>
+      </c>
+      <c r="J275" t="b">
+        <v>0</v>
+      </c>
+      <c r="K275" t="b">
+        <v>1</v>
+      </c>
+      <c r="L275" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:12" ht="18">
+      <c r="A276">
+        <v>275</v>
+      </c>
+      <c r="B276" t="s">
+        <v>1400</v>
+      </c>
+      <c r="C276">
+        <v>10</v>
+      </c>
+      <c r="D276">
+        <v>5</v>
+      </c>
+      <c r="E276" t="s">
+        <v>1401</v>
+      </c>
+      <c r="F276" t="b">
+        <v>0</v>
+      </c>
+      <c r="G276" t="s">
+        <v>1402</v>
+      </c>
+      <c r="H276" t="b">
+        <v>1</v>
+      </c>
+      <c r="I276" t="s">
+        <v>1403</v>
+      </c>
+      <c r="J276" t="b">
+        <v>0</v>
+      </c>
+      <c r="K276" s="2" t="s">
+        <v>1404</v>
+      </c>
+      <c r="L276" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:12" ht="18">
+      <c r="A277">
+        <v>276</v>
+      </c>
+      <c r="B277" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C277">
+        <v>10</v>
+      </c>
+      <c r="D277">
+        <v>6</v>
+      </c>
+      <c r="E277" t="s">
+        <v>1406</v>
+      </c>
+      <c r="F277" t="b">
+        <v>1</v>
+      </c>
+      <c r="G277" t="s">
+        <v>1407</v>
+      </c>
+      <c r="H277" t="b">
+        <v>0</v>
+      </c>
+      <c r="I277" t="s">
+        <v>1408</v>
+      </c>
+      <c r="J277" t="b">
+        <v>0</v>
+      </c>
+      <c r="K277" s="2" t="s">
+        <v>1409</v>
+      </c>
+      <c r="L277" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:12" ht="18">
+      <c r="A278">
+        <v>277</v>
+      </c>
+      <c r="B278" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C278">
+        <v>10</v>
+      </c>
+      <c r="D278">
+        <v>7</v>
+      </c>
+      <c r="E278" t="s">
+        <v>1411</v>
+      </c>
+      <c r="F278" t="b">
+        <v>0</v>
+      </c>
+      <c r="G278" t="s">
+        <v>1412</v>
+      </c>
+      <c r="H278" t="b">
+        <v>0</v>
+      </c>
+      <c r="I278" t="s">
+        <v>1413</v>
+      </c>
+      <c r="J278" t="b">
+        <v>1</v>
+      </c>
+      <c r="K278" s="2" t="s">
+        <v>1414</v>
+      </c>
+      <c r="L278" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:12" ht="18">
+      <c r="A279">
+        <v>278</v>
+      </c>
+      <c r="B279" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C279">
+        <v>10</v>
+      </c>
+      <c r="D279">
+        <v>8</v>
+      </c>
+      <c r="E279" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F279" t="b">
+        <v>0</v>
+      </c>
+      <c r="G279" t="s">
+        <v>1417</v>
+      </c>
+      <c r="H279" t="b">
+        <v>0</v>
+      </c>
+      <c r="I279" t="s">
+        <v>1418</v>
+      </c>
+      <c r="J279" t="b">
+        <v>0</v>
+      </c>
+      <c r="K279" s="2" t="s">
+        <v>1419</v>
+      </c>
+      <c r="L279" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="280" spans="1:12" ht="18">
+      <c r="A280">
+        <v>279</v>
+      </c>
+      <c r="B280" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C280">
+        <v>10</v>
+      </c>
+      <c r="D280">
+        <v>9</v>
+      </c>
+      <c r="E280" t="s">
+        <v>1421</v>
+      </c>
+      <c r="F280" t="b">
+        <v>1</v>
+      </c>
+      <c r="G280" t="s">
+        <v>1422</v>
+      </c>
+      <c r="H280" t="b">
+        <v>0</v>
+      </c>
+      <c r="I280" t="s">
+        <v>1423</v>
+      </c>
+      <c r="J280" t="b">
+        <v>0</v>
+      </c>
+      <c r="K280" s="2" t="s">
+        <v>1424</v>
+      </c>
+      <c r="L280" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:12" ht="18">
+      <c r="A281">
+        <v>280</v>
+      </c>
+      <c r="B281" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C281">
+        <v>10</v>
+      </c>
+      <c r="D281">
+        <v>10</v>
+      </c>
+      <c r="E281" t="s">
+        <v>1426</v>
+      </c>
+      <c r="F281" t="b">
+        <v>0</v>
+      </c>
+      <c r="G281" t="s">
+        <v>1427</v>
+      </c>
+      <c r="H281" t="b">
+        <v>1</v>
+      </c>
+      <c r="I281" t="s">
+        <v>1428</v>
+      </c>
+      <c r="J281" t="b">
+        <v>0</v>
+      </c>
+      <c r="K281" s="2" t="s">
+        <v>1429</v>
+      </c>
+      <c r="L281" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:12" ht="18">
+      <c r="A282">
+        <v>281</v>
+      </c>
+      <c r="B282" t="s">
+        <v>1372</v>
+      </c>
+      <c r="C282">
+        <v>10</v>
+      </c>
+      <c r="D282">
+        <v>10</v>
+      </c>
+      <c r="E282" t="s">
+        <v>1373</v>
+      </c>
+      <c r="F282" t="b">
+        <v>0</v>
+      </c>
+      <c r="G282" t="s">
+        <v>1374</v>
+      </c>
+      <c r="H282" t="b">
+        <v>1</v>
+      </c>
+      <c r="I282" t="s">
+        <v>1375</v>
+      </c>
+      <c r="J282" t="b">
+        <v>0</v>
+      </c>
+      <c r="K282" s="2" t="s">
+        <v>1376</v>
+      </c>
+      <c r="L282" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:12" ht="18">
+      <c r="A283">
+        <v>282</v>
+      </c>
+      <c r="B283" t="s">
+        <v>1386</v>
+      </c>
+      <c r="C283">
+        <v>10</v>
+      </c>
+      <c r="D283">
+        <v>9</v>
+      </c>
+      <c r="E283" t="s">
+        <v>1387</v>
+      </c>
+      <c r="F283" t="b">
+        <v>0</v>
+      </c>
+      <c r="G283" t="s">
+        <v>1388</v>
+      </c>
+      <c r="H283" t="b">
+        <v>1</v>
+      </c>
+      <c r="I283" t="s">
+        <v>1389</v>
+      </c>
+      <c r="J283" t="b">
+        <v>0</v>
+      </c>
+      <c r="K283" s="2" t="s">
+        <v>1390</v>
+      </c>
+      <c r="L283" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:12" ht="18">
+      <c r="A284">
+        <v>283</v>
+      </c>
+      <c r="B284" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C284">
+        <v>10</v>
+      </c>
+      <c r="D284">
+        <v>8</v>
+      </c>
+      <c r="E284" t="s">
+        <v>1392</v>
+      </c>
+      <c r="F284" t="b">
+        <v>1</v>
+      </c>
+      <c r="G284" t="s">
+        <v>1393</v>
+      </c>
+      <c r="H284" t="b">
+        <v>0</v>
+      </c>
+      <c r="I284" t="s">
+        <v>1394</v>
+      </c>
+      <c r="J284" t="b">
+        <v>0</v>
+      </c>
+      <c r="K284" s="2" t="s">
+        <v>1395</v>
+      </c>
+      <c r="L284" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:12">
+      <c r="A285">
+        <v>284</v>
+      </c>
+      <c r="B285" t="s">
+        <v>1396</v>
+      </c>
+      <c r="C285">
+        <v>10</v>
+      </c>
+      <c r="D285">
+        <v>7</v>
+      </c>
+      <c r="E285" t="s">
+        <v>1397</v>
+      </c>
+      <c r="F285" t="b">
+        <v>0</v>
+      </c>
+      <c r="G285" t="s">
+        <v>1398</v>
+      </c>
+      <c r="H285" t="b">
+        <v>0</v>
+      </c>
+      <c r="I285" t="s">
+        <v>1399</v>
+      </c>
+      <c r="J285" t="b">
+        <v>0</v>
+      </c>
+      <c r="K285" t="b">
+        <v>1</v>
+      </c>
+      <c r="L285" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:12" ht="18">
+      <c r="A286">
+        <v>285</v>
+      </c>
+      <c r="B286" t="s">
+        <v>1400</v>
+      </c>
+      <c r="C286">
+        <v>10</v>
+      </c>
+      <c r="D286">
+        <v>6</v>
+      </c>
+      <c r="E286" t="s">
+        <v>1401</v>
+      </c>
+      <c r="F286" t="b">
+        <v>0</v>
+      </c>
+      <c r="G286" t="s">
+        <v>1402</v>
+      </c>
+      <c r="H286" t="b">
+        <v>1</v>
+      </c>
+      <c r="I286" t="s">
+        <v>1403</v>
+      </c>
+      <c r="J286" t="b">
+        <v>0</v>
+      </c>
+      <c r="K286" s="2" t="s">
+        <v>1404</v>
+      </c>
+      <c r="L286" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:12" ht="18">
+      <c r="A287">
+        <v>286</v>
+      </c>
+      <c r="B287" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C287">
+        <v>10</v>
+      </c>
+      <c r="D287">
+        <v>5</v>
+      </c>
+      <c r="E287" t="s">
+        <v>1406</v>
+      </c>
+      <c r="F287" t="b">
+        <v>1</v>
+      </c>
+      <c r="G287" t="s">
+        <v>1407</v>
+      </c>
+      <c r="H287" t="b">
+        <v>0</v>
+      </c>
+      <c r="I287" t="s">
+        <v>1408</v>
+      </c>
+      <c r="J287" t="b">
+        <v>0</v>
+      </c>
+      <c r="K287" s="2" t="s">
+        <v>1409</v>
+      </c>
+      <c r="L287" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:12" ht="18">
+      <c r="A288">
+        <v>287</v>
+      </c>
+      <c r="B288" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C288">
+        <v>10</v>
+      </c>
+      <c r="D288">
+        <v>4</v>
+      </c>
+      <c r="E288" t="s">
+        <v>1411</v>
+      </c>
+      <c r="F288" t="b">
+        <v>0</v>
+      </c>
+      <c r="G288" t="s">
+        <v>1412</v>
+      </c>
+      <c r="H288" t="b">
+        <v>0</v>
+      </c>
+      <c r="I288" t="s">
+        <v>1413</v>
+      </c>
+      <c r="J288" t="b">
+        <v>1</v>
+      </c>
+      <c r="K288" s="2" t="s">
+        <v>1414</v>
+      </c>
+      <c r="L288" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:12" ht="18">
+      <c r="A289">
+        <v>288</v>
+      </c>
+      <c r="B289" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C289">
+        <v>10</v>
+      </c>
+      <c r="D289">
+        <v>3</v>
+      </c>
+      <c r="E289" t="s">
+        <v>1416</v>
+      </c>
+      <c r="F289" t="b">
+        <v>0</v>
+      </c>
+      <c r="G289" t="s">
+        <v>1417</v>
+      </c>
+      <c r="H289" t="b">
+        <v>0</v>
+      </c>
+      <c r="I289" t="s">
+        <v>1418</v>
+      </c>
+      <c r="J289" t="b">
+        <v>0</v>
+      </c>
+      <c r="K289" s="2" t="s">
+        <v>1419</v>
+      </c>
+      <c r="L289" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:12" ht="18">
+      <c r="A290">
+        <v>289</v>
+      </c>
+      <c r="B290" t="s">
+        <v>1420</v>
+      </c>
+      <c r="C290">
+        <v>10</v>
+      </c>
+      <c r="D290">
+        <v>2</v>
+      </c>
+      <c r="E290" t="s">
+        <v>1421</v>
+      </c>
+      <c r="F290" t="b">
+        <v>1</v>
+      </c>
+      <c r="G290" t="s">
+        <v>1422</v>
+      </c>
+      <c r="H290" t="b">
+        <v>0</v>
+      </c>
+      <c r="I290" t="s">
+        <v>1423</v>
+      </c>
+      <c r="J290" t="b">
+        <v>0</v>
+      </c>
+      <c r="K290" s="2" t="s">
+        <v>1424</v>
+      </c>
+      <c r="L290" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:12" ht="18">
+      <c r="A291">
+        <v>290</v>
+      </c>
+      <c r="B291" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C291">
+        <v>10</v>
+      </c>
+      <c r="D291">
+        <v>1</v>
+      </c>
+      <c r="E291" t="s">
+        <v>1426</v>
+      </c>
+      <c r="F291" t="b">
+        <v>0</v>
+      </c>
+      <c r="G291" t="s">
+        <v>1427</v>
+      </c>
+      <c r="H291" t="b">
+        <v>1</v>
+      </c>
+      <c r="I291" t="s">
+        <v>1428</v>
+      </c>
+      <c r="J291" t="b">
+        <v>0</v>
+      </c>
+      <c r="K291" s="2" t="s">
+        <v>1429</v>
+      </c>
+      <c r="L291" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:12" ht="18">
+      <c r="A292">
+        <v>291</v>
+      </c>
+      <c r="B292" t="s">
+        <v>1322</v>
+      </c>
+      <c r="C292">
+        <v>9</v>
+      </c>
+      <c r="D292">
+        <v>10</v>
+      </c>
+      <c r="E292" t="s">
+        <v>1323</v>
+      </c>
+      <c r="F292" t="b">
+        <v>0</v>
+      </c>
+      <c r="G292" t="s">
+        <v>1324</v>
+      </c>
+      <c r="H292" t="b">
+        <v>0</v>
+      </c>
+      <c r="I292" t="s">
+        <v>1325</v>
+      </c>
+      <c r="J292" t="b">
+        <v>0</v>
+      </c>
+      <c r="K292" s="2" t="s">
+        <v>1326</v>
+      </c>
+      <c r="L292" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:12" ht="18">
+      <c r="A293">
+        <v>292</v>
+      </c>
+      <c r="B293" t="s">
+        <v>1327</v>
+      </c>
+      <c r="C293">
+        <v>9</v>
+      </c>
+      <c r="D293">
+        <v>9</v>
+      </c>
+      <c r="E293" t="s">
+        <v>1328</v>
+      </c>
+      <c r="F293" t="b">
+        <v>0</v>
+      </c>
+      <c r="G293" t="s">
+        <v>1329</v>
+      </c>
+      <c r="H293" t="b">
+        <v>0</v>
+      </c>
+      <c r="I293" t="s">
+        <v>1330</v>
+      </c>
+      <c r="J293" t="b">
+        <v>1</v>
+      </c>
+      <c r="K293" s="2" t="s">
+        <v>1331</v>
+      </c>
+      <c r="L293" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:12" ht="18">
+      <c r="A294">
+        <v>293</v>
+      </c>
+      <c r="B294" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C294">
+        <v>9</v>
+      </c>
+      <c r="D294">
+        <v>8</v>
+      </c>
+      <c r="E294" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F294" t="b">
+        <v>0</v>
+      </c>
+      <c r="G294" t="s">
+        <v>1334</v>
+      </c>
+      <c r="H294" t="b">
+        <v>0</v>
+      </c>
+      <c r="I294" t="s">
+        <v>1335</v>
+      </c>
+      <c r="J294" t="b">
+        <v>1</v>
+      </c>
+      <c r="K294" s="2" t="s">
+        <v>1336</v>
+      </c>
+      <c r="L294" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:12" ht="18">
+      <c r="A295">
+        <v>294</v>
+      </c>
+      <c r="B295" t="s">
+        <v>1337</v>
+      </c>
+      <c r="C295">
+        <v>9</v>
+      </c>
+      <c r="D295">
+        <v>7</v>
+      </c>
+      <c r="E295" t="s">
+        <v>1338</v>
+      </c>
+      <c r="F295" t="b">
+        <v>0</v>
+      </c>
+      <c r="G295" t="s">
+        <v>1339</v>
+      </c>
+      <c r="H295" t="b">
+        <v>1</v>
+      </c>
+      <c r="I295" t="s">
+        <v>1340</v>
+      </c>
+      <c r="J295" t="b">
+        <v>0</v>
+      </c>
+      <c r="K295" s="2" t="s">
+        <v>1341</v>
+      </c>
+      <c r="L295" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:12" ht="18">
+      <c r="A296">
+        <v>295</v>
+      </c>
+      <c r="B296" t="s">
+        <v>1342</v>
+      </c>
+      <c r="C296">
+        <v>9</v>
+      </c>
+      <c r="D296">
+        <v>6</v>
+      </c>
+      <c r="E296" t="s">
+        <v>1343</v>
+      </c>
+      <c r="F296" t="b">
+        <v>1</v>
+      </c>
+      <c r="G296" t="s">
+        <v>1344</v>
+      </c>
+      <c r="H296" t="b">
+        <v>0</v>
+      </c>
+      <c r="I296" t="s">
+        <v>1345</v>
+      </c>
+      <c r="J296" t="b">
+        <v>0</v>
+      </c>
+      <c r="K296" s="2" t="s">
+        <v>1346</v>
+      </c>
+      <c r="L296" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:12" ht="18">
+      <c r="A297">
+        <v>296</v>
+      </c>
+      <c r="B297" t="s">
+        <v>1347</v>
+      </c>
+      <c r="C297">
+        <v>9</v>
+      </c>
+      <c r="D297">
+        <v>5</v>
+      </c>
+      <c r="E297" t="s">
+        <v>1348</v>
+      </c>
+      <c r="F297" t="b">
+        <v>0</v>
+      </c>
+      <c r="G297" t="s">
+        <v>1349</v>
+      </c>
+      <c r="H297" t="b">
+        <v>1</v>
+      </c>
+      <c r="I297" t="s">
+        <v>1350</v>
+      </c>
+      <c r="J297" t="b">
+        <v>0</v>
+      </c>
+      <c r="K297" s="2" t="s">
+        <v>1351</v>
+      </c>
+      <c r="L297" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:12" ht="18">
+      <c r="A298">
+        <v>297</v>
+      </c>
+      <c r="B298" t="s">
+        <v>1352</v>
+      </c>
+      <c r="C298">
+        <v>9</v>
+      </c>
+      <c r="D298">
+        <v>4</v>
+      </c>
+      <c r="E298" t="s">
+        <v>1353</v>
+      </c>
+      <c r="F298" t="b">
+        <v>0</v>
+      </c>
+      <c r="G298" t="s">
+        <v>1354</v>
+      </c>
+      <c r="H298" t="b">
+        <v>0</v>
+      </c>
+      <c r="I298" t="s">
+        <v>1355</v>
+      </c>
+      <c r="J298" t="b">
+        <v>1</v>
+      </c>
+      <c r="K298" s="2" t="s">
+        <v>1356</v>
+      </c>
+      <c r="L298" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="299" spans="1:12" ht="18">
+      <c r="A299">
+        <v>298</v>
+      </c>
+      <c r="B299" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C299">
+        <v>9</v>
+      </c>
+      <c r="D299">
+        <v>3</v>
+      </c>
+      <c r="E299" t="s">
+        <v>1358</v>
+      </c>
+      <c r="F299" t="b">
+        <v>0</v>
+      </c>
+      <c r="G299" t="s">
+        <v>1359</v>
+      </c>
+      <c r="H299" t="b">
+        <v>0</v>
+      </c>
+      <c r="I299" t="s">
+        <v>1361</v>
+      </c>
+      <c r="J299" t="b">
+        <v>1</v>
+      </c>
+      <c r="K299" s="2" t="s">
+        <v>1360</v>
+      </c>
+      <c r="L299" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300" spans="1:12" ht="18">
+      <c r="A300">
+        <v>299</v>
+      </c>
+      <c r="B300" t="s">
+        <v>1362</v>
+      </c>
+      <c r="C300">
+        <v>9</v>
+      </c>
+      <c r="D300">
+        <v>2</v>
+      </c>
+      <c r="E300" t="s">
+        <v>1363</v>
+      </c>
+      <c r="F300" t="b">
+        <v>0</v>
+      </c>
+      <c r="G300" t="s">
+        <v>1364</v>
+      </c>
+      <c r="H300" t="b">
+        <v>1</v>
+      </c>
+      <c r="I300" t="s">
+        <v>1365</v>
+      </c>
+      <c r="J300" t="b">
+        <v>0</v>
+      </c>
+      <c r="K300" s="2" t="s">
+        <v>1366</v>
+      </c>
+      <c r="L300" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:12" ht="18">
+      <c r="A301">
+        <v>300</v>
+      </c>
+      <c r="B301" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C301">
+        <v>9</v>
+      </c>
+      <c r="D301">
+        <v>1</v>
+      </c>
+      <c r="E301" t="s">
+        <v>1368</v>
+      </c>
+      <c r="F301" t="b">
+        <v>0</v>
+      </c>
+      <c r="G301" t="s">
+        <v>1369</v>
+      </c>
+      <c r="H301" t="b">
+        <v>0</v>
+      </c>
+      <c r="I301" t="s">
+        <v>1370</v>
+      </c>
+      <c r="J301" t="b">
+        <v>1</v>
+      </c>
+      <c r="K301" s="2" t="s">
+        <v>1371</v>
+      </c>
+      <c r="L301" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>